<commit_message>
Calabrio API Process - Added trax report download xaml along with all exception handled code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\botfive\Documents\UiPath\API_Test\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\botfive\Documents\UiPath\CalabrioAPI Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54830B-4970-4CB6-BF87-0B872BE7F851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450D4BB6-7624-4FB6-AF20-A05C521CB3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>report_filename</t>
   </si>
   <si>
-    <t>C:\Users\botfive\Documents\UiPath\API_Test\Generate_Reports.xlsm</t>
-  </si>
-  <si>
     <t>start_date_for_schedule_absence</t>
   </si>
   <si>
@@ -96,11 +93,26 @@
     <t>report_filepath</t>
   </si>
   <si>
-    <t>C:\Users\botfive\Documents\UiPath\API_Test\Report_data\</t>
+    <t>Needs to be in below format
+2023-11-08</t>
   </si>
   <si>
-    <t>Needs to be in below format
-2023-11-08</t>
+    <t>C:\Users\botfive\Documents\UiPath\CalabrioAPI Process\Generate_Reports.xlsm</t>
+  </si>
+  <si>
+    <t>C:\Users\botfive\Documents\UiPath\CalabrioAPI Process\Report_data\</t>
+  </si>
+  <si>
+    <t>trax_URL</t>
+  </si>
+  <si>
+    <t>https://login-eu.calabriocloud.com/?realm=/bravo#/</t>
+  </si>
+  <si>
+    <t>Email_id</t>
+  </si>
+  <si>
+    <t>vaijayanti.patil@quantanite.com</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,6 +193,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1580,7 +1593,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1636,10 +1649,10 @@
       </c>
       <c r="B2" s="7">
         <f ca="1">TODAY()-D2</f>
-        <v>45257</v>
+        <v>45273</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1650,46 +1663,60 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="7">
         <f ca="1">TODAY()-D2</f>
-        <v>45257</v>
+        <v>45273</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7">
         <f ca="1">TODAY()-D2</f>
-        <v>45257</v>
+        <v>45273</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>